<commit_message>
add TCGA survival results
</commit_message>
<xml_diff>
--- a/figures/results/MAMA-MIA_1st-contrast.xlsx
+++ b/figures/results/MAMA-MIA_1st-contrast.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>pcr.Expert.Pyradiomics.None</t>
+          <t>pcr.Expert.BayesBP.None</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1662,16 +1662,16 @@
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>0.5389648858250754</v>
+        <v>0.5102124623007325</v>
       </c>
       <c r="I42" t="n">
-        <v>0.3677203959349249</v>
+        <v>0.342981729365634</v>
       </c>
       <c r="J42" t="n">
-        <v>0.5626413722533391</v>
+        <v>0.5427752046531666</v>
       </c>
       <c r="K42" t="n">
-        <v>0.5158025457419331</v>
+        <v>0.4941214728104237</v>
       </c>
     </row>
     <row r="43">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>pcr.Expert.Pyradiomics.None</t>
+          <t>pcr.Expert.BayesBP.None</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1691,16 +1691,16 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
-        <v>0.5676297931925894</v>
+        <v>0.551297931925894</v>
       </c>
       <c r="I43" t="n">
-        <v>0.3728480212245435</v>
+        <v>0.3733593045859485</v>
       </c>
       <c r="J43" t="n">
-        <v>0.5776066350710901</v>
+        <v>0.5774316027574321</v>
       </c>
       <c r="K43" t="n">
-        <v>0.5454886817049722</v>
+        <v>0.5286883651431034</v>
       </c>
     </row>
     <row r="44">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>pcr.Expert.Pyradiomics.None</t>
+          <t>pcr.Expert.BayesBP.None</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1720,16 +1720,16 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>0.5435965101249461</v>
+        <v>0.5103134424816889</v>
       </c>
       <c r="I44" t="n">
-        <v>0.3616450416017064</v>
+        <v>0.3553593593129143</v>
       </c>
       <c r="J44" t="n">
-        <v>0.544000430848772</v>
+        <v>0.5423982119775959</v>
       </c>
       <c r="K44" t="n">
-        <v>0.5253841445882751</v>
+        <v>0.4890252074814067</v>
       </c>
     </row>
     <row r="45">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>pcr.Expert.Pyradiomics.None</t>
+          <t>pcr.Expert.BayesBP.None</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1749,16 +1749,16 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>0.5624528759155536</v>
+        <v>0.5582655644118915</v>
       </c>
       <c r="I45" t="n">
-        <v>0.3779880072141696</v>
+        <v>0.3590925995501184</v>
       </c>
       <c r="J45" t="n">
-        <v>0.5864659629470056</v>
+        <v>0.5798820551486428</v>
       </c>
       <c r="K45" t="n">
-        <v>0.5508366933739</v>
+        <v>0.5307168793979379</v>
       </c>
     </row>
     <row r="46">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>pcr.Expert.Pyradiomics.None</t>
+          <t>pcr.Expert.BayesBP.None</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1778,16 +1778,16 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
-        <v>0.5534185157259801</v>
+        <v>0.5329262710038776</v>
       </c>
       <c r="I46" t="n">
-        <v>0.3659114259168419</v>
+        <v>0.3496847410431222</v>
       </c>
       <c r="J46" t="n">
-        <v>0.5651120206807411</v>
+        <v>0.5657919538991814</v>
       </c>
       <c r="K46" t="n">
-        <v>0.5322018918123236</v>
+        <v>0.5085999832805028</v>
       </c>
     </row>
     <row r="47">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>pcr.Expert.SegVol.Mean+Max</t>
+          <t>pcr.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1807,16 +1807,16 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
-        <v>0.5111616760017235</v>
+        <v>0.5389648858250754</v>
       </c>
       <c r="I47" t="n">
-        <v>0.3005964415206969</v>
+        <v>0.3677203959349249</v>
       </c>
       <c r="J47" t="n">
-        <v>0.5106231150366222</v>
+        <v>0.5626413722533391</v>
       </c>
       <c r="K47" t="n">
-        <v>0.4899575877738772</v>
+        <v>0.5158025457419331</v>
       </c>
     </row>
     <row r="48">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>pcr.Expert.SegVol.Mean+Max</t>
+          <t>pcr.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1836,16 +1836,16 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>0.5496351249461439</v>
+        <v>0.5676297931925894</v>
       </c>
       <c r="I48" t="n">
-        <v>0.3616339771100174</v>
+        <v>0.3728480212245435</v>
       </c>
       <c r="J48" t="n">
-        <v>0.563361697544162</v>
+        <v>0.5776066350710901</v>
       </c>
       <c r="K48" t="n">
-        <v>0.5288994622869032</v>
+        <v>0.5454886817049722</v>
       </c>
     </row>
     <row r="49">
@@ -1854,7 +1854,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>pcr.Expert.SegVol.Mean+Max</t>
+          <t>pcr.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1865,16 +1865,16 @@
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
-        <v>0.54313873330461</v>
+        <v>0.5435965101249461</v>
       </c>
       <c r="I49" t="n">
-        <v>0.3475529274591377</v>
+        <v>0.3616450416017064</v>
       </c>
       <c r="J49" t="n">
-        <v>0.5602515079707022</v>
+        <v>0.544000430848772</v>
       </c>
       <c r="K49" t="n">
-        <v>0.5200190378189905</v>
+        <v>0.5253841445882751</v>
       </c>
     </row>
     <row r="50">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>pcr.Expert.SegVol.Mean+Max</t>
+          <t>pcr.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1894,16 +1894,16 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>0.5047797285652735</v>
+        <v>0.5624528759155536</v>
       </c>
       <c r="I50" t="n">
-        <v>0.3078867512170704</v>
+        <v>0.3779880072141696</v>
       </c>
       <c r="J50" t="n">
-        <v>0.532542546316243</v>
+        <v>0.5864659629470056</v>
       </c>
       <c r="K50" t="n">
-        <v>0.4844809994097499</v>
+        <v>0.5508366933739</v>
       </c>
     </row>
     <row r="51">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>pcr.Expert.SegVol.Mean+Max</t>
+          <t>pcr.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1923,16 +1923,16 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>0.5272579168461871</v>
+        <v>0.5534185157259801</v>
       </c>
       <c r="I51" t="n">
-        <v>0.33230456534825</v>
+        <v>0.3659114259168419</v>
       </c>
       <c r="J51" t="n">
-        <v>0.5374973071951745</v>
+        <v>0.5651120206807411</v>
       </c>
       <c r="K51" t="n">
-        <v>0.5101757899660797</v>
+        <v>0.5322018918123236</v>
       </c>
     </row>
     <row r="52">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.Pyradiomics.None</t>
+          <t>pcr.Expert.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1952,16 +1952,16 @@
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
-        <v>0.5470298362774666</v>
+        <v>0.5111616760017235</v>
       </c>
       <c r="I52" t="n">
-        <v>0.3639503652412734</v>
+        <v>0.3005964415206969</v>
       </c>
       <c r="J52" t="n">
-        <v>0.5693531882809134</v>
+        <v>0.5106231150366222</v>
       </c>
       <c r="K52" t="n">
-        <v>0.5279608220901201</v>
+        <v>0.4899575877738772</v>
       </c>
     </row>
     <row r="53">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.Pyradiomics.None</t>
+          <t>pcr.Expert.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1981,16 +1981,16 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
-        <v>0.5534252477380439</v>
+        <v>0.5496351249461439</v>
       </c>
       <c r="I53" t="n">
-        <v>0.37267914256359</v>
+        <v>0.3616339771100174</v>
       </c>
       <c r="J53" t="n">
-        <v>0.5735472317966395</v>
+        <v>0.563361697544162</v>
       </c>
       <c r="K53" t="n">
-        <v>0.5337088114945756</v>
+        <v>0.5288994622869032</v>
       </c>
     </row>
     <row r="54">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.Pyradiomics.None</t>
+          <t>pcr.Expert.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -2010,16 +2010,16 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
-        <v>0.5419606311934511</v>
+        <v>0.54313873330461</v>
       </c>
       <c r="I54" t="n">
-        <v>0.3693344237513143</v>
+        <v>0.3475529274591377</v>
       </c>
       <c r="J54" t="n">
-        <v>0.5374434510986643</v>
+        <v>0.5602515079707022</v>
       </c>
       <c r="K54" t="n">
-        <v>0.5262670947744713</v>
+        <v>0.5200190378189905</v>
       </c>
     </row>
     <row r="55">
@@ -2028,7 +2028,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.Pyradiomics.None</t>
+          <t>pcr.Expert.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -2039,16 +2039,16 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
-        <v>0.5464845433003016</v>
+        <v>0.5047797285652735</v>
       </c>
       <c r="I55" t="n">
-        <v>0.3623176854286065</v>
+        <v>0.3078867512170704</v>
       </c>
       <c r="J55" t="n">
-        <v>0.5636848341232228</v>
+        <v>0.532542546316243</v>
       </c>
       <c r="K55" t="n">
-        <v>0.5295967580943298</v>
+        <v>0.4844809994097499</v>
       </c>
     </row>
     <row r="56">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.Pyradiomics.None</t>
+          <t>pcr.Expert.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -2068,16 +2068,16 @@
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
-        <v>0.517664799655321</v>
+        <v>0.5272579168461871</v>
       </c>
       <c r="I56" t="n">
-        <v>0.3440536948518682</v>
+        <v>0.33230456534825</v>
       </c>
       <c r="J56" t="n">
-        <v>0.5281667384747953</v>
+        <v>0.5374973071951745</v>
       </c>
       <c r="K56" t="n">
-        <v>0.5015861722336026</v>
+        <v>0.5101757899660797</v>
       </c>
     </row>
     <row r="57">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.SegVol.Mean+Max</t>
+          <t>pcr.nnUNet.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2097,16 +2097,16 @@
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>0.52050570874623</v>
+        <v>0.5470298362774666</v>
       </c>
       <c r="I57" t="n">
-        <v>0.3188800677696095</v>
+        <v>0.3639503652412734</v>
       </c>
       <c r="J57" t="n">
-        <v>0.5196709392503231</v>
+        <v>0.5693531882809134</v>
       </c>
       <c r="K57" t="n">
-        <v>0.5043502421813291</v>
+        <v>0.5279608220901201</v>
       </c>
     </row>
     <row r="58">
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.SegVol.Mean+Max</t>
+          <t>pcr.nnUNet.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2126,16 +2126,16 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>0.5491504200775528</v>
+        <v>0.5534252477380439</v>
       </c>
       <c r="I58" t="n">
-        <v>0.3737722487519601</v>
+        <v>0.37267914256359</v>
       </c>
       <c r="J58" t="n">
-        <v>0.5731769711331323</v>
+        <v>0.5735472317966395</v>
       </c>
       <c r="K58" t="n">
-        <v>0.5261294621780855</v>
+        <v>0.5337088114945756</v>
       </c>
     </row>
     <row r="59">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.SegVol.Mean+Max</t>
+          <t>pcr.nnUNet.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -2155,16 +2155,16 @@
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
-        <v>0.5541455730288669</v>
+        <v>0.5419606311934511</v>
       </c>
       <c r="I59" t="n">
-        <v>0.3696669403922654</v>
+        <v>0.3693344237513143</v>
       </c>
       <c r="J59" t="n">
-        <v>0.5663103188280914</v>
+        <v>0.5374434510986643</v>
       </c>
       <c r="K59" t="n">
-        <v>0.5348679723070487</v>
+        <v>0.5262670947744713</v>
       </c>
     </row>
     <row r="60">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.SegVol.Mean+Max</t>
+          <t>pcr.nnUNet.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -2184,16 +2184,16 @@
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>0.5276079814735029</v>
+        <v>0.5464845433003016</v>
       </c>
       <c r="I60" t="n">
-        <v>0.317177500468635</v>
+        <v>0.3623176854286065</v>
       </c>
       <c r="J60" t="n">
-        <v>0.5418327229642395</v>
+        <v>0.5636848341232228</v>
       </c>
       <c r="K60" t="n">
-        <v>0.5077554423608285</v>
+        <v>0.5295967580943298</v>
       </c>
     </row>
     <row r="61">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>pcr.nnUNet.SegVol.Mean+Max</t>
+          <t>pcr.nnUNet.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -2213,16 +2213,16 @@
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>0.5385205730288669</v>
+        <v>0.517664799655321</v>
       </c>
       <c r="I61" t="n">
-        <v>0.3661994984744983</v>
+        <v>0.3440536948518682</v>
       </c>
       <c r="J61" t="n">
-        <v>0.5385205730288668</v>
+        <v>0.5281667384747953</v>
       </c>
       <c r="K61" t="n">
-        <v>0.5258817830779483</v>
+        <v>0.5015861722336026</v>
       </c>
     </row>
     <row r="62">
@@ -2231,28 +2231,28 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>recurrence.BiomedParse.Pyradiomics.None</t>
+          <t>pcr.nnUNet.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
-      <c r="D62" t="n">
-        <v>0.7116115029842648</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0.7951017053292965</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0.147935949225264</v>
-      </c>
-      <c r="G62" t="n">
-        <v>0.7313422551046883</v>
-      </c>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
-      <c r="J62" t="inlineStr"/>
-      <c r="K62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="n">
+        <v>0.52050570874623</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.3188800677696095</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.5196709392503231</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.5043502421813291</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2260,28 +2260,28 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>recurrence.BiomedParse.Pyradiomics.None</t>
+          <t>pcr.nnUNet.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C63" t="n">
         <v>1</v>
       </c>
-      <c r="D63" t="n">
-        <v>0.6217334494773519</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.5586896044554652</v>
-      </c>
-      <c r="F63" t="n">
-        <v>0.1527414591828133</v>
-      </c>
-      <c r="G63" t="n">
-        <v>0.6496565141380947</v>
-      </c>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
-      <c r="K63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="n">
+        <v>0.5491504200775528</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.3737722487519601</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.5731769711331323</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.5261294621780855</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2289,28 +2289,28 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>recurrence.BiomedParse.Pyradiomics.None</t>
+          <t>pcr.nnUNet.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C64" t="n">
         <v>2</v>
       </c>
-      <c r="D64" t="n">
-        <v>0.6545812254075323</v>
-      </c>
-      <c r="E64" t="n">
-        <v>0.6007459125959493</v>
-      </c>
-      <c r="F64" t="n">
-        <v>0.1550612869079236</v>
-      </c>
-      <c r="G64" t="n">
-        <v>0.68558373183004</v>
-      </c>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
-      <c r="J64" t="inlineStr"/>
-      <c r="K64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="n">
+        <v>0.5541455730288669</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.3696669403922654</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.5663103188280914</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.5348679723070487</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2318,28 +2318,28 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>recurrence.BiomedParse.Pyradiomics.None</t>
+          <t>pcr.nnUNet.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C65" t="n">
         <v>3</v>
       </c>
-      <c r="D65" t="n">
-        <v>0.5533942558746736</v>
-      </c>
-      <c r="E65" t="n">
-        <v>0.5816647251431695</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0.1619324685315564</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0.5527248807456656</v>
-      </c>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
-      <c r="J65" t="inlineStr"/>
-      <c r="K65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="n">
+        <v>0.5276079814735029</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.317177500468635</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.5418327229642395</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.5077554423608285</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2347,28 +2347,28 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>recurrence.BiomedParse.Pyradiomics.None</t>
+          <t>pcr.nnUNet.SegVol.Mean+Max</t>
         </is>
       </c>
       <c r="C66" t="n">
         <v>4</v>
       </c>
-      <c r="D66" t="n">
-        <v>0.6780957079427726</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0.6975866543398193</v>
-      </c>
-      <c r="F66" t="n">
-        <v>0.1532107707833946</v>
-      </c>
-      <c r="G66" t="n">
-        <v>0.6801936651120857</v>
-      </c>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
-      <c r="J66" t="inlineStr"/>
-      <c r="K66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="n">
+        <v>0.5385205730288669</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.3661994984744983</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.5385205730288668</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.5258817830779483</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2376,23 +2376,23 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>recurrence.Expert.Pyradiomics.None</t>
+          <t>recurrence.BiomedParse.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C67" t="n">
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>0.7316196418882257</v>
+        <v>0.7116115029842648</v>
       </c>
       <c r="E67" t="n">
-        <v>0.809838004052615</v>
+        <v>0.7951017053292965</v>
       </c>
       <c r="F67" t="n">
-        <v>0.1466615518572335</v>
+        <v>0.147935949225264</v>
       </c>
       <c r="G67" t="n">
-        <v>0.7447208258714068</v>
+        <v>0.7313422551046883</v>
       </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
@@ -2405,23 +2405,23 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>recurrence.Expert.Pyradiomics.None</t>
+          <t>recurrence.BiomedParse.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C68" t="n">
         <v>1</v>
       </c>
       <c r="D68" t="n">
-        <v>0.6421312427409989</v>
+        <v>0.6217334494773519</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5367706363218661</v>
+        <v>0.5586896044554652</v>
       </c>
       <c r="F68" t="n">
-        <v>0.1485168207685639</v>
+        <v>0.1527414591828133</v>
       </c>
       <c r="G68" t="n">
-        <v>0.675657661397393</v>
+        <v>0.6496565141380947</v>
       </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
@@ -2434,23 +2434,23 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>recurrence.Expert.Pyradiomics.None</t>
+          <t>recurrence.BiomedParse.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C69" t="n">
         <v>2</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6963884204609331</v>
+        <v>0.6545812254075323</v>
       </c>
       <c r="E69" t="n">
-        <v>0.6272379004963462</v>
+        <v>0.6007459125959493</v>
       </c>
       <c r="F69" t="n">
-        <v>0.150538086149779</v>
+        <v>0.1550612869079236</v>
       </c>
       <c r="G69" t="n">
-        <v>0.7220305932473439</v>
+        <v>0.68558373183004</v>
       </c>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
@@ -2463,23 +2463,23 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>recurrence.Expert.Pyradiomics.None</t>
+          <t>recurrence.BiomedParse.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C70" t="n">
         <v>3</v>
       </c>
       <c r="D70" t="n">
-        <v>0.5878590078328981</v>
+        <v>0.5533942558746736</v>
       </c>
       <c r="E70" t="n">
-        <v>0.6188530106308598</v>
+        <v>0.5816647251431695</v>
       </c>
       <c r="F70" t="n">
-        <v>0.1557176255199274</v>
+        <v>0.1619324685315564</v>
       </c>
       <c r="G70" t="n">
-        <v>0.5904003144108533</v>
+        <v>0.5527248807456656</v>
       </c>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
@@ -2492,23 +2492,23 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>recurrence.Expert.Pyradiomics.None</t>
+          <t>recurrence.BiomedParse.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C71" t="n">
         <v>4</v>
       </c>
       <c r="D71" t="n">
-        <v>0.6970276270350271</v>
+        <v>0.6780957079427726</v>
       </c>
       <c r="E71" t="n">
-        <v>0.7123820134201095</v>
+        <v>0.6975866543398193</v>
       </c>
       <c r="F71" t="n">
-        <v>0.1524014560080177</v>
+        <v>0.1532107707833946</v>
       </c>
       <c r="G71" t="n">
-        <v>0.7117666058940145</v>
+        <v>0.6801936651120857</v>
       </c>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
@@ -2521,23 +2521,23 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>recurrence.nnUNet.Pyradiomics.None</t>
+          <t>recurrence.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C72" t="n">
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>0.705371676614216</v>
+        <v>0.7316196418882257</v>
       </c>
       <c r="E72" t="n">
-        <v>0.7838488096005384</v>
+        <v>0.809838004052615</v>
       </c>
       <c r="F72" t="n">
-        <v>0.1478455108952721</v>
+        <v>0.1466615518572335</v>
       </c>
       <c r="G72" t="n">
-        <v>0.724224062685156</v>
+        <v>0.7447208258714068</v>
       </c>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
@@ -2550,23 +2550,23 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>recurrence.nnUNet.Pyradiomics.None</t>
+          <t>recurrence.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C73" t="n">
         <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>0.6279036004645761</v>
+        <v>0.6421312427409989</v>
       </c>
       <c r="E73" t="n">
-        <v>0.5365392635432398</v>
+        <v>0.5367706363218661</v>
       </c>
       <c r="F73" t="n">
-        <v>0.1484192169396941</v>
+        <v>0.1485168207685639</v>
       </c>
       <c r="G73" t="n">
-        <v>0.6625266651361427</v>
+        <v>0.675657661397393</v>
       </c>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
@@ -2579,23 +2579,23 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>recurrence.nnUNet.Pyradiomics.None</t>
+          <t>recurrence.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C74" t="n">
         <v>2</v>
       </c>
       <c r="D74" t="n">
-        <v>0.6224704890387858</v>
+        <v>0.6963884204609331</v>
       </c>
       <c r="E74" t="n">
-        <v>0.6025011995266066</v>
+        <v>0.6272379004963462</v>
       </c>
       <c r="F74" t="n">
-        <v>0.1589413771804402</v>
+        <v>0.150538086149779</v>
       </c>
       <c r="G74" t="n">
-        <v>0.647630075721773</v>
+        <v>0.7220305932473439</v>
       </c>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
@@ -2608,23 +2608,23 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>recurrence.nnUNet.Pyradiomics.None</t>
+          <t>recurrence.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C75" t="n">
         <v>3</v>
       </c>
       <c r="D75" t="n">
-        <v>0.5933420365535248</v>
+        <v>0.5878590078328981</v>
       </c>
       <c r="E75" t="n">
-        <v>0.6329745878258806</v>
+        <v>0.6188530106308598</v>
       </c>
       <c r="F75" t="n">
-        <v>0.1534236832000209</v>
+        <v>0.1557176255199274</v>
       </c>
       <c r="G75" t="n">
-        <v>0.5996788283788006</v>
+        <v>0.5904003144108533</v>
       </c>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
@@ -2637,29 +2637,174 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>recurrence.nnUNet.Pyradiomics.None</t>
+          <t>recurrence.Expert.Pyradiomics.None</t>
         </is>
       </c>
       <c r="C76" t="n">
         <v>4</v>
       </c>
       <c r="D76" t="n">
-        <v>0.703317710902812</v>
+        <v>0.6970276270350271</v>
       </c>
       <c r="E76" t="n">
-        <v>0.7203057291306033</v>
+        <v>0.7123820134201095</v>
       </c>
       <c r="F76" t="n">
-        <v>0.1547029639248001</v>
+        <v>0.1524014560080177</v>
       </c>
       <c r="G76" t="n">
-        <v>0.7129629297683577</v>
+        <v>0.7117666058940145</v>
       </c>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
     </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>recurrence.nnUNet.Pyradiomics.None</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.705371676614216</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.7838488096005384</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.1478455108952721</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.724224062685156</v>
+      </c>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>recurrence.nnUNet.Pyradiomics.None</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.6279036004645761</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.5365392635432398</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.1484192169396941</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.6625266651361427</v>
+      </c>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>recurrence.nnUNet.Pyradiomics.None</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>2</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.6224704890387858</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.6025011995266066</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.1589413771804402</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.647630075721773</v>
+      </c>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>recurrence.nnUNet.Pyradiomics.None</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>3</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.5933420365535248</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.6329745878258806</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.1534236832000209</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.5996788283788006</v>
+      </c>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>recurrence.nnUNet.Pyradiomics.None</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>4</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.703317710902812</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.7203057291306033</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.1547029639248001</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.7129629297683577</v>
+      </c>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>